<commit_message>
successfully send the file is done
</commit_message>
<xml_diff>
--- a/proj1/backend/login_data.xlsx
+++ b/proj1/backend/login_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Subhash\Documents\GitHub\Chat-Platform-Over-LAN\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a962fe10262e272/Documents/GitHub/Chat-Platform-Over-LAN/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7AFB71-23E2-49B7-AE34-1EA63A5198E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{BC7AFB71-23E2-49B7-AE34-1EA63A5198E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C22925B-5405-4E56-955C-FFE7CB1B0C07}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Subhash Kumar Mehta</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>a#a</t>
   </si>
 </sst>
 </file>
@@ -383,9 +386,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -425,6 +430,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>